<commit_message>
Complete list chooser added
</commit_message>
<xml_diff>
--- a/lab2/ДЗ4.xlsx
+++ b/lab2/ДЗ4.xlsx
@@ -8,28 +8,38 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Документы\GitHub\lab2\lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3317BE14-5F33-4C96-BEF3-39B349EDB164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172DEEF5-7866-43C6-986E-BC68E65FC5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Вариант 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Вариант 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Вариант 3" sheetId="3" r:id="rId3"/>
-    <sheet name="Вариант 4" sheetId="4" r:id="rId4"/>
-    <sheet name="Вариант 5" sheetId="5" r:id="rId5"/>
-    <sheet name="Вариант 6" sheetId="6" r:id="rId6"/>
-    <sheet name="Вариант 7" sheetId="7" r:id="rId7"/>
-    <sheet name="Вариант 8" sheetId="8" r:id="rId8"/>
-    <sheet name="Вариант 9" sheetId="9" r:id="rId9"/>
-    <sheet name="Вариант 10" sheetId="10" r:id="rId10"/>
+    <sheet name="Лист1" sheetId="11" r:id="rId2"/>
+    <sheet name="Вариант 2" sheetId="2" r:id="rId3"/>
+    <sheet name="Вариант 3" sheetId="3" r:id="rId4"/>
+    <sheet name="Вариант 4" sheetId="4" r:id="rId5"/>
+    <sheet name="Вариант 5" sheetId="5" r:id="rId6"/>
+    <sheet name="Вариант 6" sheetId="6" r:id="rId7"/>
+    <sheet name="Вариант 7" sheetId="7" r:id="rId8"/>
+    <sheet name="Вариант 8" sheetId="8" r:id="rId9"/>
+    <sheet name="Вариант 9" sheetId="9" r:id="rId10"/>
+    <sheet name="Вариант 10" sheetId="10" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="3">
   <si>
     <t>X</t>
   </si>
@@ -413,1123 +423,716 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:B88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.2010675985366106</v>
       </c>
       <c r="B2">
         <v>0.17872514550558477</v>
       </c>
-      <c r="C2">
-        <v>1.8310918809148982</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.23135439958423376</v>
       </c>
       <c r="B3">
         <v>0.75483310285806515</v>
       </c>
-      <c r="C3">
-        <v>-2.6269987996408721</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>7.1375269442796707E-2</v>
       </c>
       <c r="B4">
         <v>0.51495574013251166</v>
       </c>
-      <c r="C4">
-        <v>4.2304046738688372</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.3390725958161056</v>
       </c>
       <c r="B5">
         <v>0.54183437278053159</v>
       </c>
-      <c r="C5">
-        <v>1.066782941013757</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-0.47738726064562798</v>
       </c>
       <c r="B6">
         <v>0.72871702646285874</v>
       </c>
-      <c r="C6">
-        <v>0.43287870376676185</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9.73875867202878E-3</v>
       </c>
       <c r="B7">
         <v>0.67016163346551161</v>
       </c>
-      <c r="C7">
-        <v>-1.1635636434458561</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-0.21327780000865459</v>
       </c>
       <c r="B8">
         <v>0.6211359828403169</v>
       </c>
-      <c r="C8">
-        <v>-0.56938300998238045</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.39354863530024886</v>
       </c>
       <c r="B9">
         <v>0.66725186613288945</v>
       </c>
-      <c r="C9">
-        <v>7.1002919494284438</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-0.43338972143828869</v>
       </c>
       <c r="B10">
         <v>0.98264332297178825</v>
       </c>
-      <c r="C10">
-        <v>3.2797827515244053</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.92699490021914244</v>
       </c>
       <c r="B11">
         <v>0.72644477296746124</v>
       </c>
-      <c r="C11">
-        <v>3.1028778237201529</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.44358324073255062</v>
       </c>
       <c r="B12">
         <v>0.45517617287480494</v>
       </c>
-      <c r="C12">
-        <v>1.5064273030259421</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>-2.6568260975182056E-2</v>
       </c>
       <c r="B13">
         <v>0.49035308576837811</v>
       </c>
-      <c r="C13">
-        <v>4.8677608592970403</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.51652928395196795</v>
       </c>
       <c r="B14">
         <v>0.44777232634037289</v>
       </c>
-      <c r="C14">
-        <v>8.7392233711144645</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.52675847196951509</v>
       </c>
       <c r="B15">
         <v>0.56561769793625682</v>
       </c>
-      <c r="C15">
-        <v>6.2917556366794161</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.9335155226290226</v>
       </c>
       <c r="B16">
         <v>0.57502563137035223</v>
       </c>
-      <c r="C16">
-        <v>2.424949130006302</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-4.6884305775165558E-3</v>
       </c>
       <c r="B17">
         <v>0.68053177948101018</v>
       </c>
-      <c r="C17">
-        <v>0.88771051431395653</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>-0.70669449027627707</v>
       </c>
       <c r="B18">
         <v>0.70192336474882988</v>
       </c>
-      <c r="C18">
-        <v>0.7283029470290161</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>-0.15904274675995111</v>
       </c>
       <c r="B19">
         <v>0.68208664850365253</v>
       </c>
-      <c r="C19">
-        <v>0.59141411684614753</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-8.0294620245695114E-2</v>
       </c>
       <c r="B20">
         <v>0.79964861826524103</v>
       </c>
-      <c r="C20">
-        <v>1.8340839878336068</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0.4499690355733037</v>
       </c>
       <c r="B21">
         <v>0.39383724488320115</v>
       </c>
-      <c r="C21">
-        <v>3.3510765763627108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>-0.13071688171476126</v>
       </c>
       <c r="B22">
         <v>0.81907989613805388</v>
       </c>
-      <c r="C22">
-        <v>-0.17745770148050433</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>-0.13668572995811701</v>
       </c>
       <c r="B23">
         <v>0.51940971682913872</v>
       </c>
-      <c r="C23">
-        <v>3.6236549709822832</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.29431003471836448</v>
       </c>
       <c r="B24">
         <v>0.69437688937287745</v>
       </c>
-      <c r="C24">
-        <v>0.56366095750393441</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0.90488147456198931</v>
       </c>
       <c r="B25">
         <v>0.57467695851623524</v>
       </c>
-      <c r="C25">
-        <v>3.9677264723983718</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>5.7924873661249876E-2</v>
       </c>
       <c r="B26">
         <v>0.65118880288212244</v>
       </c>
-      <c r="C26">
-        <v>1.1804755701555458</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0.43523160833865404</v>
       </c>
       <c r="B27">
         <v>0.4952633872902234</v>
       </c>
-      <c r="C27">
-        <v>-0.97672326035259927</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>-0.49092343542724848</v>
       </c>
       <c r="B28">
         <v>0.11844759971404351</v>
       </c>
-      <c r="C28">
-        <v>-2.9173839685832395</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0.84821080742403865</v>
       </c>
       <c r="B29">
         <v>0.87806060103231309</v>
       </c>
-      <c r="C29">
-        <v>-0.47481295092781561</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0.55495384335517883</v>
       </c>
       <c r="B30">
         <v>0.57164050679244804</v>
       </c>
-      <c r="C30">
-        <v>-0.12527680151999387</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0.62150189047679305</v>
       </c>
       <c r="B31">
         <v>0.89281946686152214</v>
       </c>
-      <c r="C31">
-        <v>6.4672012628429503</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0.37478847894817591</v>
       </c>
       <c r="B32">
         <v>0.78063212784872038</v>
       </c>
-      <c r="C32">
-        <v>10.625527530777841</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>-0.87289016600698233</v>
       </c>
       <c r="B33">
         <v>0.48907672473706809</v>
       </c>
-      <c r="C33">
-        <v>4.2049465423043673</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0.42230975860729814</v>
       </c>
       <c r="B34">
         <v>0.34047211946695261</v>
       </c>
-      <c r="C34">
-        <v>7.3290793444674014</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>-0.65396047104150057</v>
       </c>
       <c r="B35">
         <v>0.41116187114475744</v>
       </c>
-      <c r="C35">
-        <v>-1.5781218264538346</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0.76975664496421814</v>
       </c>
       <c r="B36">
         <v>0.46444693159771866</v>
       </c>
-      <c r="C36">
-        <v>1.7856243297128052</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0.1977199986577034</v>
       </c>
       <c r="B37">
         <v>0.58343200535775275</v>
       </c>
-      <c r="C37">
-        <v>5.3433602359335559</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0.63818094925954938</v>
       </c>
       <c r="B38">
         <v>0.58328734630399004</v>
       </c>
-      <c r="C38">
-        <v>2.5808112110278021</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>-0.76401986833661795</v>
       </c>
       <c r="B39">
         <v>0.99171133895398289</v>
       </c>
-      <c r="C39">
-        <v>-0.52003450687211306</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>-0.12037713220342994</v>
       </c>
       <c r="B40">
         <v>0.6590187865048639</v>
       </c>
-      <c r="C40">
-        <v>-2.2573444304640091</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0.32050846377387643</v>
       </c>
       <c r="B41">
         <v>0.73012609123906214</v>
       </c>
-      <c r="C41">
-        <v>0.68503936766228057</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0.19054241897538304</v>
       </c>
       <c r="B42">
         <v>0.57708109294155707</v>
       </c>
-      <c r="C42">
-        <v>1.0940447659578996</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0.2856798991560936</v>
       </c>
       <c r="B43">
         <v>0.61924232276650304</v>
       </c>
-      <c r="C43">
-        <v>-0.44295866357647595</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>-0.76402369001880288</v>
       </c>
       <c r="B44">
         <v>0.71523356887446687</v>
       </c>
-      <c r="C44">
-        <v>-0.35282634621240616</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>0.31588512007147074</v>
       </c>
       <c r="B45">
         <v>0.43428837707444501</v>
       </c>
-      <c r="C45">
-        <v>6.00738692020877</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>0.18359604803845286</v>
       </c>
       <c r="B46">
         <v>0.44694631449550187</v>
       </c>
-      <c r="C46">
-        <v>3.1980232919261149</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>-0.7048473609611392</v>
       </c>
       <c r="B47">
         <v>0.92569389443034023</v>
       </c>
-      <c r="C47">
-        <v>-0.8832615827547472</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>-0.56083495076745749</v>
       </c>
       <c r="B48">
         <v>0.40172503911663127</v>
       </c>
-      <c r="C48">
-        <v>3.7396343491419222</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>-0.99503191513940692</v>
       </c>
       <c r="B49">
         <v>0.45589147165466298</v>
       </c>
-      <c r="C49">
-        <v>4.4546644063718501</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>0.58127150591462851</v>
       </c>
       <c r="B50">
         <v>0.47764496068221068</v>
       </c>
-      <c r="C50">
-        <v>3.8126510391176596</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>7.4637843295931816E-2</v>
       </c>
       <c r="B51">
         <v>0.89640915302974988</v>
       </c>
-      <c r="C51">
-        <v>9.5503641905407353</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>-0.33827040391042829</v>
       </c>
       <c r="B52">
         <v>0.5398579184906146</v>
       </c>
-      <c r="C52">
-        <v>-0.62035768533098601</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>0.43169908225536346</v>
       </c>
       <c r="B53">
         <v>0.4500480305147761</v>
       </c>
-      <c r="C53">
-        <v>4.1157036839557897</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>-0.5653578476049006</v>
       </c>
       <c r="B54">
         <v>0.84170995803143456</v>
       </c>
-      <c r="C54">
-        <v>5.6660530948232495</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>-0.53881968930363655</v>
       </c>
       <c r="B55">
         <v>0.18368211010228797</v>
       </c>
-      <c r="C55">
-        <v>1.8123857600629421</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>-0.7724966979585588</v>
       </c>
       <c r="B56">
         <v>0.43423935840879546</v>
       </c>
-      <c r="C56">
-        <v>5.3381210980090454</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>0.63429681584239006</v>
       </c>
       <c r="B57">
         <v>0.59023298680753022</v>
       </c>
-      <c r="C57">
-        <v>8.0328605779759599</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>0.98327357228845358</v>
       </c>
       <c r="B58">
         <v>0.65559991826932673</v>
       </c>
-      <c r="C58">
-        <v>1.0725012607378603</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>0.56763219460844994</v>
       </c>
       <c r="B59">
         <v>0.80938093960530899</v>
       </c>
-      <c r="C59">
-        <v>0.75405890307751644</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>-0.30725612957030535</v>
       </c>
       <c r="B60">
         <v>0.50492657384568751</v>
       </c>
-      <c r="C60">
-        <v>0.74832582772551182</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>-7.9632940702140331E-2</v>
       </c>
       <c r="B61">
         <v>0.69659901707874006</v>
       </c>
-      <c r="C61">
-        <v>7.857826687452274E-2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>0.91470761736854911</v>
       </c>
       <c r="B62">
         <v>0.76253077941116154</v>
       </c>
-      <c r="C62">
-        <v>3.6123836452847726</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>-0.40727846976369619</v>
       </c>
       <c r="B63">
         <v>0.82308076465995827</v>
       </c>
-      <c r="C63">
-        <v>3.6536782007785975</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>8.9888463262468576E-2</v>
       </c>
       <c r="B64">
         <v>0.86221653648815044</v>
       </c>
-      <c r="C64">
-        <v>0.77948085409610579</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>0.5055894972756505</v>
       </c>
       <c r="B65">
         <v>0.56460403702362105</v>
       </c>
-      <c r="C65">
-        <v>-2.021303908438286</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>-0.16490439837798476</v>
       </c>
       <c r="B66">
         <v>0.35589399900308194</v>
       </c>
-      <c r="C66">
-        <v>7.6064301053833336</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>-0.67842119000852108</v>
       </c>
       <c r="B67">
         <v>0.49211875909326952</v>
       </c>
-      <c r="C67">
-        <v>0.52510312040041396</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>-0.12185006402432919</v>
       </c>
       <c r="B68">
         <v>0.68396722321411296</v>
       </c>
-      <c r="C68">
-        <v>-7.2612369088196793E-2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>-0.14148544333875179</v>
       </c>
       <c r="B69">
         <v>0.74551134401149577</v>
       </c>
-      <c r="C69">
-        <v>1.6539009227648929</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>0.62157277623191476</v>
       </c>
       <c r="B70">
         <v>0.24881206998739308</v>
       </c>
-      <c r="C70">
-        <v>5.3928267658002547</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>0.35467028943821788</v>
       </c>
       <c r="B71">
         <v>0.89699528188081779</v>
       </c>
-      <c r="C71">
-        <v>3.578008080715656</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>-0.64234098047018051</v>
       </c>
       <c r="B72">
         <v>0.13360888506395341</v>
       </c>
-      <c r="C72">
-        <v>-0.35955906252572811</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>0.14277811395004392</v>
       </c>
       <c r="B73">
         <v>0.71339977797820608</v>
       </c>
-      <c r="C73">
-        <v>3.4537737192587414</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>-0.68164190743118525</v>
       </c>
       <c r="B74">
         <v>0.69147098793897277</v>
       </c>
-      <c r="C74">
-        <v>6.1513758648181858</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>0.22331226291134953</v>
       </c>
       <c r="B75">
         <v>0.52784676030140509</v>
       </c>
-      <c r="C75">
-        <v>2.3814567551082577</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>0.96807686006650329</v>
       </c>
       <c r="B76">
         <v>0.83628237761876334</v>
       </c>
-      <c r="C76">
-        <v>3.7195676701998717</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>-0.43599451659247279</v>
       </c>
       <c r="B77">
         <v>9.216914351260054E-2</v>
       </c>
-      <c r="C77">
-        <v>-2.1408507708198545</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>0.57387520978227258</v>
       </c>
       <c r="B78">
         <v>0.63729595242605597</v>
       </c>
-      <c r="C78">
-        <v>1.2185839199218615</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>0.94270908460021019</v>
       </c>
       <c r="B79">
         <v>0.79754029310410179</v>
       </c>
-      <c r="C79">
-        <v>-0.49806247811866289</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>-0.99210325255990028</v>
       </c>
       <c r="B80">
         <v>0.45550343325544973</v>
       </c>
-      <c r="C80">
-        <v>-2.2787659366105641</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>0.85317451599985361</v>
       </c>
       <c r="B81">
         <v>0.30251210629407854</v>
       </c>
-      <c r="C81">
-        <v>3.7869595653712209</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>-0.7052529095672071</v>
       </c>
       <c r="B82">
         <v>0.20193682736282836</v>
       </c>
-      <c r="C82">
-        <v>-1.345962717440353</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>0.38789858715608716</v>
       </c>
       <c r="B83">
         <v>0.93206876587262466</v>
       </c>
-      <c r="C83">
-        <v>0.32553199437815339</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>-0.99291521357372403</v>
       </c>
       <c r="B84">
         <v>0.61886123167285756</v>
       </c>
-      <c r="C84">
-        <v>0.51315920187731612</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>-7.6939624268561602E-2</v>
       </c>
       <c r="B85">
         <v>0.85553178537399144</v>
       </c>
-      <c r="C85">
-        <v>-1.2749890052493633</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>0.60053574293851852</v>
       </c>
       <c r="B86">
         <v>0.75274480800326904</v>
       </c>
-      <c r="C86">
-        <v>2.7786054053724709</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>-3.8831955287605524E-2</v>
       </c>
       <c r="B87">
         <v>0.51966182314213538</v>
       </c>
-      <c r="C87">
-        <v>1.681062604634789</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>0.86713533662259579</v>
       </c>
       <c r="B88">
         <v>0.43511299348857679</v>
-      </c>
-      <c r="C88">
-        <v>-3.9137531981865763</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>-0.60107270814478397</v>
-      </c>
-      <c r="B89">
-        <v>0.16538861298933591</v>
-      </c>
-      <c r="C89">
-        <v>2.1686287793905805</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <v>-0.81047396920621395</v>
-      </c>
-      <c r="B90">
-        <v>0.72821439653913411</v>
-      </c>
-      <c r="C90">
-        <v>4.9159151811495061</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>0.97810417134314775</v>
-      </c>
-      <c r="B91">
-        <v>0.38822132127139392</v>
-      </c>
-      <c r="C91">
-        <v>7.1398630755790649</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>0.7791461693122983</v>
-      </c>
-      <c r="B92">
-        <v>0.39533227613030791</v>
-      </c>
-      <c r="C92">
-        <v>7.3035091686749238</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>0.58903424814343452</v>
-      </c>
-      <c r="B93">
-        <v>0.86732985350944836</v>
-      </c>
-      <c r="C93">
-        <v>-0.57946803390050494</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>0.4973145998083055</v>
-      </c>
-      <c r="B94">
-        <v>0.91512650939177698</v>
-      </c>
-      <c r="C94">
-        <v>9.0850171798761981E-2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>0.69323321944102645</v>
-      </c>
-      <c r="B95">
-        <v>0.26301919286720454</v>
-      </c>
-      <c r="C95">
-        <v>-0.35736035578147263</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>0.47046097414568067</v>
-      </c>
-      <c r="B96">
-        <v>0.74554613906155476</v>
-      </c>
-      <c r="C96">
-        <v>4.2237477984314786</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <v>-5.3820788860321045E-2</v>
-      </c>
-      <c r="B97">
-        <v>0.49732694157576252</v>
-      </c>
-      <c r="C97">
-        <v>-0.8665057894231234</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>-0.48259945353493094</v>
-      </c>
-      <c r="B98">
-        <v>0.5856828075665278</v>
-      </c>
-      <c r="C98">
-        <v>2.3385154557391985</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>-0.89401011355221272</v>
-      </c>
-      <c r="B99">
-        <v>0.70659107248754505</v>
-      </c>
-      <c r="C99">
-        <v>4.3012200343987557</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>0.79421565029770136</v>
-      </c>
-      <c r="B100">
-        <v>0.66595604961134813</v>
-      </c>
-      <c r="C100">
-        <v>3.3513261738873776</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <v>-0.18472275882959366</v>
-      </c>
-      <c r="B101">
-        <v>0.872801107461329</v>
-      </c>
-      <c r="C101">
-        <v>6.4278862835417607</v>
       </c>
     </row>
   </sheetData>
@@ -1538,6 +1141,1435 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:D101"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.39140210440382361</v>
+      </c>
+      <c r="B2">
+        <v>0.1314685811268092</v>
+      </c>
+      <c r="C2">
+        <v>-2.8260091280246424</v>
+      </c>
+      <c r="D2">
+        <v>-2.8260091280246424</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>-0.52229759097099304</v>
+      </c>
+      <c r="B3">
+        <v>0.42658953591609083</v>
+      </c>
+      <c r="C3">
+        <v>4.6350964440527456</v>
+      </c>
+      <c r="D3">
+        <v>4.6350964440527456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.87596849771216512</v>
+      </c>
+      <c r="B4">
+        <v>0.93081474579186152</v>
+      </c>
+      <c r="C4">
+        <v>5.1018912259927447</v>
+      </c>
+      <c r="D4">
+        <v>5.1018912259927447</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>-0.39618555177003145</v>
+      </c>
+      <c r="B5">
+        <v>0.38757397586923104</v>
+      </c>
+      <c r="C5">
+        <v>3.3428177087788331</v>
+      </c>
+      <c r="D5">
+        <v>3.3428177087788331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.19210502086207271</v>
+      </c>
+      <c r="B6">
+        <v>0.66259287765014385</v>
+      </c>
+      <c r="C6">
+        <v>-0.76432712954066995</v>
+      </c>
+      <c r="D6">
+        <v>-0.76432712954066995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>-0.95668709138408303</v>
+      </c>
+      <c r="B7">
+        <v>0.70931910727173131</v>
+      </c>
+      <c r="C7">
+        <v>1.4273319113501595</v>
+      </c>
+      <c r="D7">
+        <v>1.4273319113501595</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-0.10449800547212362</v>
+      </c>
+      <c r="B8">
+        <v>0.13138381303977559</v>
+      </c>
+      <c r="C8">
+        <v>3.6362081593478628</v>
+      </c>
+      <c r="D8">
+        <v>3.6362081593478628</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>-0.11936450283974409</v>
+      </c>
+      <c r="B9">
+        <v>0.78454056434958064</v>
+      </c>
+      <c r="C9">
+        <v>3.4473538332223832</v>
+      </c>
+      <c r="D9">
+        <v>3.4473538332223832</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>-0.99875800916925073</v>
+      </c>
+      <c r="B10">
+        <v>0.10603395472056616</v>
+      </c>
+      <c r="C10">
+        <v>2.1515889369843015</v>
+      </c>
+      <c r="D10">
+        <v>2.1515889369843015</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.63034723000600934</v>
+      </c>
+      <c r="B11">
+        <v>0.13990233927000076</v>
+      </c>
+      <c r="C11">
+        <v>3.7728574446203478</v>
+      </c>
+      <c r="D11">
+        <v>3.7728574446203478</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.47276790346950293</v>
+      </c>
+      <c r="B12">
+        <v>0.5631075285141145</v>
+      </c>
+      <c r="C12">
+        <v>-1.282294628285519</v>
+      </c>
+      <c r="D12">
+        <v>-1.282294628285519</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.11342388717457652</v>
+      </c>
+      <c r="B13">
+        <v>0.71676830766458133</v>
+      </c>
+      <c r="C13">
+        <v>-1.7345299047445857</v>
+      </c>
+      <c r="D13">
+        <v>-1.7345299047445857</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-0.57745106145739555</v>
+      </c>
+      <c r="B14">
+        <v>0.55821835813563514</v>
+      </c>
+      <c r="C14">
+        <v>6.4794794073601638</v>
+      </c>
+      <c r="D14">
+        <v>6.4794794073601638</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.67914127837866545</v>
+      </c>
+      <c r="B15">
+        <v>0.30409618152724749</v>
+      </c>
+      <c r="C15">
+        <v>1.552634031417726</v>
+      </c>
+      <c r="D15">
+        <v>1.552634031417726</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5.958501435816288E-2</v>
+      </c>
+      <c r="B16">
+        <v>0.50869226234673648</v>
+      </c>
+      <c r="C16">
+        <v>2.2140103691205852</v>
+      </c>
+      <c r="D16">
+        <v>2.2140103691205852</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>-0.38707641931250691</v>
+      </c>
+      <c r="B17">
+        <v>0.43935577133584292</v>
+      </c>
+      <c r="C17">
+        <v>0.41751709831185657</v>
+      </c>
+      <c r="D17">
+        <v>0.41751709831185657</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>-0.83702964661642909</v>
+      </c>
+      <c r="B18">
+        <v>0.27056428752087058</v>
+      </c>
+      <c r="C18">
+        <v>-3.2379741543094109</v>
+      </c>
+      <c r="D18">
+        <v>-3.2379741543094109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.65515548037365079</v>
+      </c>
+      <c r="B19">
+        <v>0.47555308341966651</v>
+      </c>
+      <c r="C19">
+        <v>3.9855633943663351</v>
+      </c>
+      <c r="D19">
+        <v>3.9855633943663351</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3.3400805201381445E-2</v>
+      </c>
+      <c r="B20">
+        <v>0.67957372296055463</v>
+      </c>
+      <c r="C20">
+        <v>3.2276156201710213</v>
+      </c>
+      <c r="D20">
+        <v>3.2276156201710213</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.3311811862513423</v>
+      </c>
+      <c r="B21">
+        <v>0.89216681764402572</v>
+      </c>
+      <c r="C21">
+        <v>-0.42746404903037449</v>
+      </c>
+      <c r="D21">
+        <v>-0.42746404903037449</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.71859577530995011</v>
+      </c>
+      <c r="B22">
+        <v>0.37805499074447341</v>
+      </c>
+      <c r="C22">
+        <v>5.2661104937783101</v>
+      </c>
+      <c r="D22">
+        <v>5.2661104937783101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.74123864201828837</v>
+      </c>
+      <c r="B23">
+        <v>0.78578494341245098</v>
+      </c>
+      <c r="C23">
+        <v>-1.7106159363592646</v>
+      </c>
+      <c r="D23">
+        <v>-1.7106159363592646</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>-0.8732299767434597</v>
+      </c>
+      <c r="B24">
+        <v>0.90177099125504279</v>
+      </c>
+      <c r="C24">
+        <v>2.7105987936029194</v>
+      </c>
+      <c r="D24">
+        <v>2.7105987936029194</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.62222181027755141</v>
+      </c>
+      <c r="B25">
+        <v>0.57553287564148292</v>
+      </c>
+      <c r="C25">
+        <v>0.75413604083939045</v>
+      </c>
+      <c r="D25">
+        <v>0.75413604083939045</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>-0.36937455274164677</v>
+      </c>
+      <c r="B26">
+        <v>0.48660974640102622</v>
+      </c>
+      <c r="C26">
+        <v>4.1874143905808552</v>
+      </c>
+      <c r="D26">
+        <v>4.1874143905808552</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>-0.49581704987213016</v>
+      </c>
+      <c r="B27">
+        <v>0.90203356768097764</v>
+      </c>
+      <c r="C27">
+        <v>0.80486478245879445</v>
+      </c>
+      <c r="D27">
+        <v>0.80486478245879445</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>-8.108448563143611E-2</v>
+      </c>
+      <c r="B28">
+        <v>0.56727914111285427</v>
+      </c>
+      <c r="C28">
+        <v>4.7972344695383082</v>
+      </c>
+      <c r="D28">
+        <v>4.7972344695383082</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>-0.15617561992257833</v>
+      </c>
+      <c r="B29">
+        <v>0.73131823243966532</v>
+      </c>
+      <c r="C29">
+        <v>2.3326981384444707</v>
+      </c>
+      <c r="D29">
+        <v>2.3326981384444707</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>-0.57730586780235171</v>
+      </c>
+      <c r="B30">
+        <v>0.35489333172932497</v>
+      </c>
+      <c r="C30">
+        <v>7.2983474444391527</v>
+      </c>
+      <c r="D30">
+        <v>7.2983474444391527</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0.26373649341985583</v>
+      </c>
+      <c r="B31">
+        <v>0.34223195075705798</v>
+      </c>
+      <c r="C31">
+        <v>3.6071446872258628</v>
+      </c>
+      <c r="D31">
+        <v>3.6071446872258628</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0.90585017530247569</v>
+      </c>
+      <c r="B32">
+        <v>0.71561675846202499</v>
+      </c>
+      <c r="C32">
+        <v>3.4794922342984416</v>
+      </c>
+      <c r="D32">
+        <v>3.4794922342984416</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0.45024189213290811</v>
+      </c>
+      <c r="B33">
+        <v>0.19723940416049926</v>
+      </c>
+      <c r="C33">
+        <v>1.006034030706098</v>
+      </c>
+      <c r="D33">
+        <v>1.006034030706098</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>-0.47372684022411704</v>
+      </c>
+      <c r="B34">
+        <v>0.44639804593827037</v>
+      </c>
+      <c r="C34">
+        <v>1.1782001064040803</v>
+      </c>
+      <c r="D34">
+        <v>1.1782001064040803</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>-0.69152020802721381</v>
+      </c>
+      <c r="B35">
+        <v>0.61687639236993574</v>
+      </c>
+      <c r="C35">
+        <v>2.0504877685972462</v>
+      </c>
+      <c r="D35">
+        <v>2.0504877685972462</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>0.86951710097491741</v>
+      </c>
+      <c r="B36">
+        <v>0.4643776941929938</v>
+      </c>
+      <c r="C36">
+        <v>8.9104237557629418E-2</v>
+      </c>
+      <c r="D36">
+        <v>8.9104237557629418E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>-0.6761753698810935</v>
+      </c>
+      <c r="B37">
+        <v>0.86884068055804742</v>
+      </c>
+      <c r="C37">
+        <v>7.4463058894026064</v>
+      </c>
+      <c r="D37">
+        <v>7.4463058894026064</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>0.53931050049141049</v>
+      </c>
+      <c r="B38">
+        <v>0.45126250242136673</v>
+      </c>
+      <c r="C38">
+        <v>1.307264922986223</v>
+      </c>
+      <c r="D38">
+        <v>1.307264922986223</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>0.31303410418331623</v>
+      </c>
+      <c r="B39">
+        <v>0.69712292681630206</v>
+      </c>
+      <c r="C39">
+        <v>6.2342496314924833</v>
+      </c>
+      <c r="D39">
+        <v>6.2342496314924833</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>0.35185526311397552</v>
+      </c>
+      <c r="B40">
+        <v>0.40012311775245674</v>
+      </c>
+      <c r="C40">
+        <v>-4.0200048687260459</v>
+      </c>
+      <c r="D40">
+        <v>-4.0200048687260459</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>0.89112694095820189</v>
+      </c>
+      <c r="B41">
+        <v>0.5976110446039441</v>
+      </c>
+      <c r="C41">
+        <v>3.4169148835772045E-2</v>
+      </c>
+      <c r="D41">
+        <v>3.4169148835772045E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>-0.27256935695186257</v>
+      </c>
+      <c r="B42">
+        <v>0.41851314442873155</v>
+      </c>
+      <c r="C42">
+        <v>-1.3548335789010286</v>
+      </c>
+      <c r="D42">
+        <v>-1.3548335789010286</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>0.33053294010460377</v>
+      </c>
+      <c r="B43">
+        <v>0.4062008328090409</v>
+      </c>
+      <c r="C43">
+        <v>-1.1596026423635903</v>
+      </c>
+      <c r="D43">
+        <v>-1.1596026423635903</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>-0.29519950738176703</v>
+      </c>
+      <c r="B44">
+        <v>0.15969717775198106</v>
+      </c>
+      <c r="C44">
+        <v>1.0305361356862546</v>
+      </c>
+      <c r="D44">
+        <v>1.0305361356862546</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>-0.1013447567820549</v>
+      </c>
+      <c r="B45">
+        <v>0.82141603718974421</v>
+      </c>
+      <c r="C45">
+        <v>-3.4377109086470448</v>
+      </c>
+      <c r="D45">
+        <v>-3.4377109086470448</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>0.14390164194628596</v>
+      </c>
+      <c r="B46">
+        <v>0.68631523009428574</v>
+      </c>
+      <c r="C46">
+        <v>2.4622699294033259</v>
+      </c>
+      <c r="D46">
+        <v>2.4622699294033259</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>-0.47559220204129815</v>
+      </c>
+      <c r="B47">
+        <v>0.74566376220042918</v>
+      </c>
+      <c r="C47">
+        <v>-0.99732039943250061</v>
+      </c>
+      <c r="D47">
+        <v>-0.99732039943250061</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>0.61171672400087118</v>
+      </c>
+      <c r="B48">
+        <v>6.7854623536600725E-2</v>
+      </c>
+      <c r="C48">
+        <v>1.1005746032064949</v>
+      </c>
+      <c r="D48">
+        <v>1.1005746032064949</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>0.27816094411537051</v>
+      </c>
+      <c r="B49">
+        <v>0.82585167005802462</v>
+      </c>
+      <c r="C49">
+        <v>6.5988649374727313</v>
+      </c>
+      <c r="D49">
+        <v>6.5988649374727313</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>-0.90146514819934964</v>
+      </c>
+      <c r="B50">
+        <v>0.10993521648427924</v>
+      </c>
+      <c r="C50">
+        <v>-0.20768759448005492</v>
+      </c>
+      <c r="D50">
+        <v>-0.20768759448005492</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>-0.69292904064059258</v>
+      </c>
+      <c r="B51">
+        <v>0.35936908160203057</v>
+      </c>
+      <c r="C51">
+        <v>5.7701361645018228</v>
+      </c>
+      <c r="D51">
+        <v>5.7701361645018228</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>-0.32952900836244226</v>
+      </c>
+      <c r="B52">
+        <v>0.4644778809840136</v>
+      </c>
+      <c r="C52">
+        <v>5.5068435364648307</v>
+      </c>
+      <c r="D52">
+        <v>5.5068435364648307</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>0.33525006379932165</v>
+      </c>
+      <c r="B53">
+        <v>0.71609005148339189</v>
+      </c>
+      <c r="C53">
+        <v>4.55777452279745</v>
+      </c>
+      <c r="D53">
+        <v>4.55777452279745</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>0.42683249805122614</v>
+      </c>
+      <c r="B54">
+        <v>0.87204465417089594</v>
+      </c>
+      <c r="C54">
+        <v>1.7655618709339955</v>
+      </c>
+      <c r="D54">
+        <v>1.7655618709339955</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>9.628297109156847E-2</v>
+      </c>
+      <c r="B55">
+        <v>0.74054380062048408</v>
+      </c>
+      <c r="C55">
+        <v>2.8929635328363386</v>
+      </c>
+      <c r="D55">
+        <v>2.8929635328363386</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>-0.86457695998251438</v>
+      </c>
+      <c r="B56">
+        <v>0.35552563999353248</v>
+      </c>
+      <c r="C56">
+        <v>-1.3746628318613956</v>
+      </c>
+      <c r="D56">
+        <v>-1.3746628318613956</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>0.58661293378099799</v>
+      </c>
+      <c r="B57">
+        <v>0.38615562622748251</v>
+      </c>
+      <c r="C57">
+        <v>2.3641003336061077</v>
+      </c>
+      <c r="D57">
+        <v>2.3641003336061077</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>0.61329979356378317</v>
+      </c>
+      <c r="B58">
+        <v>0.63748594686477589</v>
+      </c>
+      <c r="C58">
+        <v>-0.2242246965670307</v>
+      </c>
+      <c r="D58">
+        <v>-0.2242246965670307</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>0.57989999745041132</v>
+      </c>
+      <c r="B59">
+        <v>0.24676979074511346</v>
+      </c>
+      <c r="C59">
+        <v>2.3702425359557728</v>
+      </c>
+      <c r="D59">
+        <v>2.3702425359557728</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>-0.29786984389647841</v>
+      </c>
+      <c r="B60">
+        <v>0.7138753976497223</v>
+      </c>
+      <c r="C60">
+        <v>-1.7621347660757678</v>
+      </c>
+      <c r="D60">
+        <v>-1.7621347660757678</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>-0.25192663352936506</v>
+      </c>
+      <c r="B61">
+        <v>0.50399007519296113</v>
+      </c>
+      <c r="C61">
+        <v>1.6284041941724754</v>
+      </c>
+      <c r="D61">
+        <v>1.6284041941724754</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>0.48018350452184677</v>
+      </c>
+      <c r="B62">
+        <v>0.28839783695296578</v>
+      </c>
+      <c r="C62">
+        <v>1.3172492959891171</v>
+      </c>
+      <c r="D62">
+        <v>1.3172492959891171</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>-0.29192132456228137</v>
+      </c>
+      <c r="B63">
+        <v>0.78861790975567847</v>
+      </c>
+      <c r="C63">
+        <v>5.654164964431482</v>
+      </c>
+      <c r="D63">
+        <v>5.654164964431482</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>-0.91082127671688795</v>
+      </c>
+      <c r="B64">
+        <v>0.61678229362504644</v>
+      </c>
+      <c r="C64">
+        <v>2.8889448734743386</v>
+      </c>
+      <c r="D64">
+        <v>2.8889448734743386</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>0.34804622549563646</v>
+      </c>
+      <c r="B65">
+        <v>0.50807573787328897</v>
+      </c>
+      <c r="C65">
+        <v>2.748629263631813</v>
+      </c>
+      <c r="D65">
+        <v>2.748629263631813</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>-0.43176339287310839</v>
+      </c>
+      <c r="B66">
+        <v>0.51533682376554879</v>
+      </c>
+      <c r="C66">
+        <v>4.0799376584670313</v>
+      </c>
+      <c r="D66">
+        <v>4.0799376584670313</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>0.40278653148561716</v>
+      </c>
+      <c r="B67">
+        <v>0.55979050475122705</v>
+      </c>
+      <c r="C67">
+        <v>1.1364009938133222</v>
+      </c>
+      <c r="D67">
+        <v>1.1364009938133222</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>-0.26215709280222654</v>
+      </c>
+      <c r="B68">
+        <v>0.32770115272872663</v>
+      </c>
+      <c r="C68">
+        <v>-2.6311626294112642</v>
+      </c>
+      <c r="D68">
+        <v>-2.6311626294112642</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>-0.46861377684399486</v>
+      </c>
+      <c r="B69">
+        <v>0.62609376310019749</v>
+      </c>
+      <c r="C69">
+        <v>-0.5669105660389766</v>
+      </c>
+      <c r="D69">
+        <v>-0.5669105660389766</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>0.93003437900915742</v>
+      </c>
+      <c r="B70">
+        <v>0.73212371148153066</v>
+      </c>
+      <c r="C70">
+        <v>0.12861105403616291</v>
+      </c>
+      <c r="D70">
+        <v>0.12861105403616291</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>0.80312925251200795</v>
+      </c>
+      <c r="B71">
+        <v>0.27723276185663853</v>
+      </c>
+      <c r="C71">
+        <v>-0.65976582412958029</v>
+      </c>
+      <c r="D71">
+        <v>-0.65976582412958029</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>-0.68696849793195724</v>
+      </c>
+      <c r="B72">
+        <v>0.85646519989367853</v>
+      </c>
+      <c r="C72">
+        <v>2.4321500942923606</v>
+      </c>
+      <c r="D72">
+        <v>2.4321500942923606</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>-0.6590762953273952</v>
+      </c>
+      <c r="B73">
+        <v>0.87030137716759659</v>
+      </c>
+      <c r="C73">
+        <v>6.3744434583225544</v>
+      </c>
+      <c r="D73">
+        <v>6.3744434583225544</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>0.3168933866545558</v>
+      </c>
+      <c r="B74">
+        <v>0.88745993806447188</v>
+      </c>
+      <c r="C74">
+        <v>2.8505365823561846</v>
+      </c>
+      <c r="D74">
+        <v>2.8505365823561846</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>0.60784284537658095</v>
+      </c>
+      <c r="B75">
+        <v>0.71701165218701191</v>
+      </c>
+      <c r="C75">
+        <v>1.5461745982230135</v>
+      </c>
+      <c r="D75">
+        <v>1.5461745982230135</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>-0.59493754617869854</v>
+      </c>
+      <c r="B76">
+        <v>0.50830310050459138</v>
+      </c>
+      <c r="C76">
+        <v>2.3491970193892695</v>
+      </c>
+      <c r="D76">
+        <v>2.3491970193892695</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>0.27055360563099384</v>
+      </c>
+      <c r="B77">
+        <v>0.61967795842667939</v>
+      </c>
+      <c r="C77">
+        <v>1.8487862557860726</v>
+      </c>
+      <c r="D77">
+        <v>1.8487862557860726</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>-0.10009184200316668</v>
+      </c>
+      <c r="B78">
+        <v>0.24006192989349837</v>
+      </c>
+      <c r="C78">
+        <v>1.1935708685451325</v>
+      </c>
+      <c r="D78">
+        <v>1.1935708685451325</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>0.79606163268908858</v>
+      </c>
+      <c r="B79">
+        <v>0.45599108148897033</v>
+      </c>
+      <c r="C79">
+        <v>2.4149826706961917</v>
+      </c>
+      <c r="D79">
+        <v>2.4149826706961917</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>-0.33815954113379121</v>
+      </c>
+      <c r="B80">
+        <v>0.85066148317167645</v>
+      </c>
+      <c r="C80">
+        <v>5.1969840339901987</v>
+      </c>
+      <c r="D80">
+        <v>5.1969840339901987</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>-0.25958700757473707</v>
+      </c>
+      <c r="B81">
+        <v>0.60215006583329755</v>
+      </c>
+      <c r="C81">
+        <v>-1.9021269811673447</v>
+      </c>
+      <c r="D81">
+        <v>-1.9021269811673447</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>0.6611259076744318</v>
+      </c>
+      <c r="B82">
+        <v>0.74189061213826046</v>
+      </c>
+      <c r="C82">
+        <v>3.5767110282390639</v>
+      </c>
+      <c r="D82">
+        <v>3.5767110282390639</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>-0.4177185851149261</v>
+      </c>
+      <c r="B83">
+        <v>0.37432048000845114</v>
+      </c>
+      <c r="C83">
+        <v>1.1545554672128397</v>
+      </c>
+      <c r="D83">
+        <v>1.1545554672128397</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>0.62532191211357713</v>
+      </c>
+      <c r="B84">
+        <v>0.61941352062909771</v>
+      </c>
+      <c r="C84">
+        <v>-1.9089264363352179</v>
+      </c>
+      <c r="D84">
+        <v>-1.9089264363352179</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>0.28010437684133649</v>
+      </c>
+      <c r="B85">
+        <v>0.11187126962852734</v>
+      </c>
+      <c r="C85">
+        <v>4.1383001919165139</v>
+      </c>
+      <c r="D85">
+        <v>4.1383001919165139</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>0.37171070743352175</v>
+      </c>
+      <c r="B86">
+        <v>0.22914502905569734</v>
+      </c>
+      <c r="C86">
+        <v>-0.73538181680084413</v>
+      </c>
+      <c r="D86">
+        <v>-0.73538181680084413</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>-2.3498728405684233E-2</v>
+      </c>
+      <c r="B87">
+        <v>0.83423183832299708</v>
+      </c>
+      <c r="C87">
+        <v>6.1520467110905814</v>
+      </c>
+      <c r="D87">
+        <v>6.1520467110905814</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>0.36598141398280859</v>
+      </c>
+      <c r="B88">
+        <v>0.36052129017813928</v>
+      </c>
+      <c r="C88">
+        <v>3.0652817896660673</v>
+      </c>
+      <c r="D88">
+        <v>3.0652817896660673</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>-0.73137106746435165</v>
+      </c>
+      <c r="B89">
+        <v>0.9523209941081725</v>
+      </c>
+      <c r="C89">
+        <v>-1.2541605097835546</v>
+      </c>
+      <c r="D89">
+        <v>-1.2541605097835546</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>6.6931700333952904E-2</v>
+      </c>
+      <c r="B90">
+        <v>0.33932080191803249</v>
+      </c>
+      <c r="C90">
+        <v>2.8154014222675272</v>
+      </c>
+      <c r="D90">
+        <v>2.8154014222675272</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>0.50061998516321182</v>
+      </c>
+      <c r="B91">
+        <v>0.58717582933158641</v>
+      </c>
+      <c r="C91">
+        <v>3.0275562573791142</v>
+      </c>
+      <c r="D91">
+        <v>3.0275562573791142</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>0.25722116138786077</v>
+      </c>
+      <c r="B92">
+        <v>0.67185143525285274</v>
+      </c>
+      <c r="C92">
+        <v>5.6486916454667258</v>
+      </c>
+      <c r="D92">
+        <v>5.6486916454667258</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>-0.32637759391218424</v>
+      </c>
+      <c r="B93">
+        <v>0.65143113937539654</v>
+      </c>
+      <c r="C93">
+        <v>3.829135001119909</v>
+      </c>
+      <c r="D93">
+        <v>3.829135001119909</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>-0.801655865740031</v>
+      </c>
+      <c r="B94">
+        <v>0.37540367192598789</v>
+      </c>
+      <c r="C94">
+        <v>7.784545404301034</v>
+      </c>
+      <c r="D94">
+        <v>7.784545404301034</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>0.79797026654705405</v>
+      </c>
+      <c r="B95">
+        <v>0.87009751405998814</v>
+      </c>
+      <c r="C95">
+        <v>-2.4411080132540901</v>
+      </c>
+      <c r="D95">
+        <v>-2.4411080132540901</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>6.05545649304986E-2</v>
+      </c>
+      <c r="B96">
+        <v>0.83226891657592039</v>
+      </c>
+      <c r="C96">
+        <v>5.7577909822258997</v>
+      </c>
+      <c r="D96">
+        <v>5.7577909822258997</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>-0.80952635360881686</v>
+      </c>
+      <c r="B97">
+        <v>0.3199582956942279</v>
+      </c>
+      <c r="C97">
+        <v>-1.4940430248515804</v>
+      </c>
+      <c r="D97">
+        <v>-1.4940430248515804</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>0.45351168466731906</v>
+      </c>
+      <c r="B98">
+        <v>0.49291685043121797</v>
+      </c>
+      <c r="C98">
+        <v>0.15100594179886162</v>
+      </c>
+      <c r="D98">
+        <v>0.15100594179886162</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>0.34591140458360314</v>
+      </c>
+      <c r="B99">
+        <v>0.38765161365002254</v>
+      </c>
+      <c r="C99">
+        <v>2.6161221467094253</v>
+      </c>
+      <c r="D99">
+        <v>2.6161221467094253</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>0.7174810110591352</v>
+      </c>
+      <c r="B100">
+        <v>0.82573982937149881</v>
+      </c>
+      <c r="C100">
+        <v>4.9221390967172383</v>
+      </c>
+      <c r="D100">
+        <v>4.9221390967172383</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>-0.94411851745098829</v>
+      </c>
+      <c r="B101">
+        <v>0.90323890173730392</v>
+      </c>
+      <c r="C101">
+        <v>4.0263725186965367</v>
+      </c>
+      <c r="D101">
+        <v>4.0263725186965367</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C101"/>
   <sheetViews>
@@ -2664,6 +3696,186 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27449FB9-E432-4F30-A2D1-F3FD49C6DF01}">
+  <dimension ref="F8:H22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="8" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>0.82077505579218268</v>
+      </c>
+      <c r="G8">
+        <v>0.47307466873793208</v>
+      </c>
+      <c r="H8">
+        <v>5.3195654402713082</v>
+      </c>
+    </row>
+    <row r="9" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>-0.67566110752522945</v>
+      </c>
+      <c r="G9">
+        <v>0.88200832058207501</v>
+      </c>
+      <c r="H9">
+        <v>-1.8842597370971772</v>
+      </c>
+    </row>
+    <row r="10" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>-0.2752647721208632</v>
+      </c>
+      <c r="G10">
+        <v>0.96629619623149388</v>
+      </c>
+      <c r="H10">
+        <v>6.4632952996068713</v>
+      </c>
+    </row>
+    <row r="11" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>-6.517201941460371E-2</v>
+      </c>
+      <c r="G11">
+        <v>0.29632666004063674</v>
+      </c>
+      <c r="H11">
+        <v>-2.5312365152762117</v>
+      </c>
+    </row>
+    <row r="12" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>0.43522558826953173</v>
+      </c>
+      <c r="G12">
+        <v>0.87768413122121369</v>
+      </c>
+      <c r="H12">
+        <v>0.5207361322444064</v>
+      </c>
+    </row>
+    <row r="13" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>0.59561238018795848</v>
+      </c>
+      <c r="G13">
+        <v>0.32942961451828712</v>
+      </c>
+      <c r="H13">
+        <v>-0.72647418813066045</v>
+      </c>
+    </row>
+    <row r="14" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>0.63590054353699088</v>
+      </c>
+      <c r="G14">
+        <v>0.62885608903734502</v>
+      </c>
+      <c r="H14">
+        <v>-2.1116380369472925</v>
+      </c>
+    </row>
+    <row r="15" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>-0.33295812923461199</v>
+      </c>
+      <c r="G15">
+        <v>0.74152770672188828</v>
+      </c>
+      <c r="H15">
+        <v>2.7378349566373705</v>
+      </c>
+    </row>
+    <row r="16" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>-0.87104257475584745</v>
+      </c>
+      <c r="G16">
+        <v>0.56882663692087165</v>
+      </c>
+      <c r="H16">
+        <v>-1.5192957348173657</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>0.40537410415709019</v>
+      </c>
+      <c r="G17">
+        <v>0.76623609241163726</v>
+      </c>
+      <c r="H17">
+        <v>3.9064496887590408</v>
+      </c>
+    </row>
+    <row r="18" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>0.12020929483696818</v>
+      </c>
+      <c r="G18">
+        <v>0.76580999517666271</v>
+      </c>
+      <c r="H18">
+        <v>0.84186366533512325</v>
+      </c>
+    </row>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>0.53950026864185929</v>
+      </c>
+      <c r="G19">
+        <v>0.65248224479566108</v>
+      </c>
+      <c r="H19">
+        <v>-3.6983436287355058</v>
+      </c>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>0.288978043012321</v>
+      </c>
+      <c r="G20">
+        <v>0.438334070848033</v>
+      </c>
+      <c r="H20">
+        <v>7.4395127835859434</v>
+      </c>
+    </row>
+    <row r="21" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>-0.72393237659707665</v>
+      </c>
+      <c r="G21">
+        <v>0.69940145972044321</v>
+      </c>
+      <c r="H21">
+        <v>2.9476620835004086</v>
+      </c>
+    </row>
+    <row r="22" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>-0.86888727964833379</v>
+      </c>
+      <c r="G22">
+        <v>0.14167736778660175</v>
+      </c>
+      <c r="H22">
+        <v>2.8536742026946977</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C101"/>
   <sheetViews>
@@ -3789,12 +5001,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4915,7 +6127,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C101"/>
   <sheetViews>
@@ -6041,7 +7253,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C101"/>
   <sheetViews>
@@ -7167,7 +8379,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C96"/>
   <sheetViews>
@@ -8130,7 +9342,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C101"/>
   <sheetViews>
@@ -9256,7 +10468,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C101"/>
   <sheetViews>
@@ -10380,1433 +11592,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D101"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0.39140210440382361</v>
-      </c>
-      <c r="B2">
-        <v>0.1314685811268092</v>
-      </c>
-      <c r="C2">
-        <v>-2.8260091280246424</v>
-      </c>
-      <c r="D2">
-        <v>-2.8260091280246424</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>-0.52229759097099304</v>
-      </c>
-      <c r="B3">
-        <v>0.42658953591609083</v>
-      </c>
-      <c r="C3">
-        <v>4.6350964440527456</v>
-      </c>
-      <c r="D3">
-        <v>4.6350964440527456</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0.87596849771216512</v>
-      </c>
-      <c r="B4">
-        <v>0.93081474579186152</v>
-      </c>
-      <c r="C4">
-        <v>5.1018912259927447</v>
-      </c>
-      <c r="D4">
-        <v>5.1018912259927447</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>-0.39618555177003145</v>
-      </c>
-      <c r="B5">
-        <v>0.38757397586923104</v>
-      </c>
-      <c r="C5">
-        <v>3.3428177087788331</v>
-      </c>
-      <c r="D5">
-        <v>3.3428177087788331</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>0.19210502086207271</v>
-      </c>
-      <c r="B6">
-        <v>0.66259287765014385</v>
-      </c>
-      <c r="C6">
-        <v>-0.76432712954066995</v>
-      </c>
-      <c r="D6">
-        <v>-0.76432712954066995</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>-0.95668709138408303</v>
-      </c>
-      <c r="B7">
-        <v>0.70931910727173131</v>
-      </c>
-      <c r="C7">
-        <v>1.4273319113501595</v>
-      </c>
-      <c r="D7">
-        <v>1.4273319113501595</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>-0.10449800547212362</v>
-      </c>
-      <c r="B8">
-        <v>0.13138381303977559</v>
-      </c>
-      <c r="C8">
-        <v>3.6362081593478628</v>
-      </c>
-      <c r="D8">
-        <v>3.6362081593478628</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>-0.11936450283974409</v>
-      </c>
-      <c r="B9">
-        <v>0.78454056434958064</v>
-      </c>
-      <c r="C9">
-        <v>3.4473538332223832</v>
-      </c>
-      <c r="D9">
-        <v>3.4473538332223832</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>-0.99875800916925073</v>
-      </c>
-      <c r="B10">
-        <v>0.10603395472056616</v>
-      </c>
-      <c r="C10">
-        <v>2.1515889369843015</v>
-      </c>
-      <c r="D10">
-        <v>2.1515889369843015</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>0.63034723000600934</v>
-      </c>
-      <c r="B11">
-        <v>0.13990233927000076</v>
-      </c>
-      <c r="C11">
-        <v>3.7728574446203478</v>
-      </c>
-      <c r="D11">
-        <v>3.7728574446203478</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>0.47276790346950293</v>
-      </c>
-      <c r="B12">
-        <v>0.5631075285141145</v>
-      </c>
-      <c r="C12">
-        <v>-1.282294628285519</v>
-      </c>
-      <c r="D12">
-        <v>-1.282294628285519</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>0.11342388717457652</v>
-      </c>
-      <c r="B13">
-        <v>0.71676830766458133</v>
-      </c>
-      <c r="C13">
-        <v>-1.7345299047445857</v>
-      </c>
-      <c r="D13">
-        <v>-1.7345299047445857</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>-0.57745106145739555</v>
-      </c>
-      <c r="B14">
-        <v>0.55821835813563514</v>
-      </c>
-      <c r="C14">
-        <v>6.4794794073601638</v>
-      </c>
-      <c r="D14">
-        <v>6.4794794073601638</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>0.67914127837866545</v>
-      </c>
-      <c r="B15">
-        <v>0.30409618152724749</v>
-      </c>
-      <c r="C15">
-        <v>1.552634031417726</v>
-      </c>
-      <c r="D15">
-        <v>1.552634031417726</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>5.958501435816288E-2</v>
-      </c>
-      <c r="B16">
-        <v>0.50869226234673648</v>
-      </c>
-      <c r="C16">
-        <v>2.2140103691205852</v>
-      </c>
-      <c r="D16">
-        <v>2.2140103691205852</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>-0.38707641931250691</v>
-      </c>
-      <c r="B17">
-        <v>0.43935577133584292</v>
-      </c>
-      <c r="C17">
-        <v>0.41751709831185657</v>
-      </c>
-      <c r="D17">
-        <v>0.41751709831185657</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>-0.83702964661642909</v>
-      </c>
-      <c r="B18">
-        <v>0.27056428752087058</v>
-      </c>
-      <c r="C18">
-        <v>-3.2379741543094109</v>
-      </c>
-      <c r="D18">
-        <v>-3.2379741543094109</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>0.65515548037365079</v>
-      </c>
-      <c r="B19">
-        <v>0.47555308341966651</v>
-      </c>
-      <c r="C19">
-        <v>3.9855633943663351</v>
-      </c>
-      <c r="D19">
-        <v>3.9855633943663351</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>3.3400805201381445E-2</v>
-      </c>
-      <c r="B20">
-        <v>0.67957372296055463</v>
-      </c>
-      <c r="C20">
-        <v>3.2276156201710213</v>
-      </c>
-      <c r="D20">
-        <v>3.2276156201710213</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>0.3311811862513423</v>
-      </c>
-      <c r="B21">
-        <v>0.89216681764402572</v>
-      </c>
-      <c r="C21">
-        <v>-0.42746404903037449</v>
-      </c>
-      <c r="D21">
-        <v>-0.42746404903037449</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>0.71859577530995011</v>
-      </c>
-      <c r="B22">
-        <v>0.37805499074447341</v>
-      </c>
-      <c r="C22">
-        <v>5.2661104937783101</v>
-      </c>
-      <c r="D22">
-        <v>5.2661104937783101</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>0.74123864201828837</v>
-      </c>
-      <c r="B23">
-        <v>0.78578494341245098</v>
-      </c>
-      <c r="C23">
-        <v>-1.7106159363592646</v>
-      </c>
-      <c r="D23">
-        <v>-1.7106159363592646</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>-0.8732299767434597</v>
-      </c>
-      <c r="B24">
-        <v>0.90177099125504279</v>
-      </c>
-      <c r="C24">
-        <v>2.7105987936029194</v>
-      </c>
-      <c r="D24">
-        <v>2.7105987936029194</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>0.62222181027755141</v>
-      </c>
-      <c r="B25">
-        <v>0.57553287564148292</v>
-      </c>
-      <c r="C25">
-        <v>0.75413604083939045</v>
-      </c>
-      <c r="D25">
-        <v>0.75413604083939045</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>-0.36937455274164677</v>
-      </c>
-      <c r="B26">
-        <v>0.48660974640102622</v>
-      </c>
-      <c r="C26">
-        <v>4.1874143905808552</v>
-      </c>
-      <c r="D26">
-        <v>4.1874143905808552</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>-0.49581704987213016</v>
-      </c>
-      <c r="B27">
-        <v>0.90203356768097764</v>
-      </c>
-      <c r="C27">
-        <v>0.80486478245879445</v>
-      </c>
-      <c r="D27">
-        <v>0.80486478245879445</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>-8.108448563143611E-2</v>
-      </c>
-      <c r="B28">
-        <v>0.56727914111285427</v>
-      </c>
-      <c r="C28">
-        <v>4.7972344695383082</v>
-      </c>
-      <c r="D28">
-        <v>4.7972344695383082</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>-0.15617561992257833</v>
-      </c>
-      <c r="B29">
-        <v>0.73131823243966532</v>
-      </c>
-      <c r="C29">
-        <v>2.3326981384444707</v>
-      </c>
-      <c r="D29">
-        <v>2.3326981384444707</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>-0.57730586780235171</v>
-      </c>
-      <c r="B30">
-        <v>0.35489333172932497</v>
-      </c>
-      <c r="C30">
-        <v>7.2983474444391527</v>
-      </c>
-      <c r="D30">
-        <v>7.2983474444391527</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>0.26373649341985583</v>
-      </c>
-      <c r="B31">
-        <v>0.34223195075705798</v>
-      </c>
-      <c r="C31">
-        <v>3.6071446872258628</v>
-      </c>
-      <c r="D31">
-        <v>3.6071446872258628</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>0.90585017530247569</v>
-      </c>
-      <c r="B32">
-        <v>0.71561675846202499</v>
-      </c>
-      <c r="C32">
-        <v>3.4794922342984416</v>
-      </c>
-      <c r="D32">
-        <v>3.4794922342984416</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>0.45024189213290811</v>
-      </c>
-      <c r="B33">
-        <v>0.19723940416049926</v>
-      </c>
-      <c r="C33">
-        <v>1.006034030706098</v>
-      </c>
-      <c r="D33">
-        <v>1.006034030706098</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>-0.47372684022411704</v>
-      </c>
-      <c r="B34">
-        <v>0.44639804593827037</v>
-      </c>
-      <c r="C34">
-        <v>1.1782001064040803</v>
-      </c>
-      <c r="D34">
-        <v>1.1782001064040803</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>-0.69152020802721381</v>
-      </c>
-      <c r="B35">
-        <v>0.61687639236993574</v>
-      </c>
-      <c r="C35">
-        <v>2.0504877685972462</v>
-      </c>
-      <c r="D35">
-        <v>2.0504877685972462</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>0.86951710097491741</v>
-      </c>
-      <c r="B36">
-        <v>0.4643776941929938</v>
-      </c>
-      <c r="C36">
-        <v>8.9104237557629418E-2</v>
-      </c>
-      <c r="D36">
-        <v>8.9104237557629418E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>-0.6761753698810935</v>
-      </c>
-      <c r="B37">
-        <v>0.86884068055804742</v>
-      </c>
-      <c r="C37">
-        <v>7.4463058894026064</v>
-      </c>
-      <c r="D37">
-        <v>7.4463058894026064</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>0.53931050049141049</v>
-      </c>
-      <c r="B38">
-        <v>0.45126250242136673</v>
-      </c>
-      <c r="C38">
-        <v>1.307264922986223</v>
-      </c>
-      <c r="D38">
-        <v>1.307264922986223</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>0.31303410418331623</v>
-      </c>
-      <c r="B39">
-        <v>0.69712292681630206</v>
-      </c>
-      <c r="C39">
-        <v>6.2342496314924833</v>
-      </c>
-      <c r="D39">
-        <v>6.2342496314924833</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>0.35185526311397552</v>
-      </c>
-      <c r="B40">
-        <v>0.40012311775245674</v>
-      </c>
-      <c r="C40">
-        <v>-4.0200048687260459</v>
-      </c>
-      <c r="D40">
-        <v>-4.0200048687260459</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>0.89112694095820189</v>
-      </c>
-      <c r="B41">
-        <v>0.5976110446039441</v>
-      </c>
-      <c r="C41">
-        <v>3.4169148835772045E-2</v>
-      </c>
-      <c r="D41">
-        <v>3.4169148835772045E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>-0.27256935695186257</v>
-      </c>
-      <c r="B42">
-        <v>0.41851314442873155</v>
-      </c>
-      <c r="C42">
-        <v>-1.3548335789010286</v>
-      </c>
-      <c r="D42">
-        <v>-1.3548335789010286</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>0.33053294010460377</v>
-      </c>
-      <c r="B43">
-        <v>0.4062008328090409</v>
-      </c>
-      <c r="C43">
-        <v>-1.1596026423635903</v>
-      </c>
-      <c r="D43">
-        <v>-1.1596026423635903</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>-0.29519950738176703</v>
-      </c>
-      <c r="B44">
-        <v>0.15969717775198106</v>
-      </c>
-      <c r="C44">
-        <v>1.0305361356862546</v>
-      </c>
-      <c r="D44">
-        <v>1.0305361356862546</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>-0.1013447567820549</v>
-      </c>
-      <c r="B45">
-        <v>0.82141603718974421</v>
-      </c>
-      <c r="C45">
-        <v>-3.4377109086470448</v>
-      </c>
-      <c r="D45">
-        <v>-3.4377109086470448</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>0.14390164194628596</v>
-      </c>
-      <c r="B46">
-        <v>0.68631523009428574</v>
-      </c>
-      <c r="C46">
-        <v>2.4622699294033259</v>
-      </c>
-      <c r="D46">
-        <v>2.4622699294033259</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>-0.47559220204129815</v>
-      </c>
-      <c r="B47">
-        <v>0.74566376220042918</v>
-      </c>
-      <c r="C47">
-        <v>-0.99732039943250061</v>
-      </c>
-      <c r="D47">
-        <v>-0.99732039943250061</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>0.61171672400087118</v>
-      </c>
-      <c r="B48">
-        <v>6.7854623536600725E-2</v>
-      </c>
-      <c r="C48">
-        <v>1.1005746032064949</v>
-      </c>
-      <c r="D48">
-        <v>1.1005746032064949</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>0.27816094411537051</v>
-      </c>
-      <c r="B49">
-        <v>0.82585167005802462</v>
-      </c>
-      <c r="C49">
-        <v>6.5988649374727313</v>
-      </c>
-      <c r="D49">
-        <v>6.5988649374727313</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>-0.90146514819934964</v>
-      </c>
-      <c r="B50">
-        <v>0.10993521648427924</v>
-      </c>
-      <c r="C50">
-        <v>-0.20768759448005492</v>
-      </c>
-      <c r="D50">
-        <v>-0.20768759448005492</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>-0.69292904064059258</v>
-      </c>
-      <c r="B51">
-        <v>0.35936908160203057</v>
-      </c>
-      <c r="C51">
-        <v>5.7701361645018228</v>
-      </c>
-      <c r="D51">
-        <v>5.7701361645018228</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>-0.32952900836244226</v>
-      </c>
-      <c r="B52">
-        <v>0.4644778809840136</v>
-      </c>
-      <c r="C52">
-        <v>5.5068435364648307</v>
-      </c>
-      <c r="D52">
-        <v>5.5068435364648307</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>0.33525006379932165</v>
-      </c>
-      <c r="B53">
-        <v>0.71609005148339189</v>
-      </c>
-      <c r="C53">
-        <v>4.55777452279745</v>
-      </c>
-      <c r="D53">
-        <v>4.55777452279745</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>0.42683249805122614</v>
-      </c>
-      <c r="B54">
-        <v>0.87204465417089594</v>
-      </c>
-      <c r="C54">
-        <v>1.7655618709339955</v>
-      </c>
-      <c r="D54">
-        <v>1.7655618709339955</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>9.628297109156847E-2</v>
-      </c>
-      <c r="B55">
-        <v>0.74054380062048408</v>
-      </c>
-      <c r="C55">
-        <v>2.8929635328363386</v>
-      </c>
-      <c r="D55">
-        <v>2.8929635328363386</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>-0.86457695998251438</v>
-      </c>
-      <c r="B56">
-        <v>0.35552563999353248</v>
-      </c>
-      <c r="C56">
-        <v>-1.3746628318613956</v>
-      </c>
-      <c r="D56">
-        <v>-1.3746628318613956</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>0.58661293378099799</v>
-      </c>
-      <c r="B57">
-        <v>0.38615562622748251</v>
-      </c>
-      <c r="C57">
-        <v>2.3641003336061077</v>
-      </c>
-      <c r="D57">
-        <v>2.3641003336061077</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>0.61329979356378317</v>
-      </c>
-      <c r="B58">
-        <v>0.63748594686477589</v>
-      </c>
-      <c r="C58">
-        <v>-0.2242246965670307</v>
-      </c>
-      <c r="D58">
-        <v>-0.2242246965670307</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>0.57989999745041132</v>
-      </c>
-      <c r="B59">
-        <v>0.24676979074511346</v>
-      </c>
-      <c r="C59">
-        <v>2.3702425359557728</v>
-      </c>
-      <c r="D59">
-        <v>2.3702425359557728</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>-0.29786984389647841</v>
-      </c>
-      <c r="B60">
-        <v>0.7138753976497223</v>
-      </c>
-      <c r="C60">
-        <v>-1.7621347660757678</v>
-      </c>
-      <c r="D60">
-        <v>-1.7621347660757678</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>-0.25192663352936506</v>
-      </c>
-      <c r="B61">
-        <v>0.50399007519296113</v>
-      </c>
-      <c r="C61">
-        <v>1.6284041941724754</v>
-      </c>
-      <c r="D61">
-        <v>1.6284041941724754</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>0.48018350452184677</v>
-      </c>
-      <c r="B62">
-        <v>0.28839783695296578</v>
-      </c>
-      <c r="C62">
-        <v>1.3172492959891171</v>
-      </c>
-      <c r="D62">
-        <v>1.3172492959891171</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>-0.29192132456228137</v>
-      </c>
-      <c r="B63">
-        <v>0.78861790975567847</v>
-      </c>
-      <c r="C63">
-        <v>5.654164964431482</v>
-      </c>
-      <c r="D63">
-        <v>5.654164964431482</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>-0.91082127671688795</v>
-      </c>
-      <c r="B64">
-        <v>0.61678229362504644</v>
-      </c>
-      <c r="C64">
-        <v>2.8889448734743386</v>
-      </c>
-      <c r="D64">
-        <v>2.8889448734743386</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>0.34804622549563646</v>
-      </c>
-      <c r="B65">
-        <v>0.50807573787328897</v>
-      </c>
-      <c r="C65">
-        <v>2.748629263631813</v>
-      </c>
-      <c r="D65">
-        <v>2.748629263631813</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>-0.43176339287310839</v>
-      </c>
-      <c r="B66">
-        <v>0.51533682376554879</v>
-      </c>
-      <c r="C66">
-        <v>4.0799376584670313</v>
-      </c>
-      <c r="D66">
-        <v>4.0799376584670313</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>0.40278653148561716</v>
-      </c>
-      <c r="B67">
-        <v>0.55979050475122705</v>
-      </c>
-      <c r="C67">
-        <v>1.1364009938133222</v>
-      </c>
-      <c r="D67">
-        <v>1.1364009938133222</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>-0.26215709280222654</v>
-      </c>
-      <c r="B68">
-        <v>0.32770115272872663</v>
-      </c>
-      <c r="C68">
-        <v>-2.6311626294112642</v>
-      </c>
-      <c r="D68">
-        <v>-2.6311626294112642</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>-0.46861377684399486</v>
-      </c>
-      <c r="B69">
-        <v>0.62609376310019749</v>
-      </c>
-      <c r="C69">
-        <v>-0.5669105660389766</v>
-      </c>
-      <c r="D69">
-        <v>-0.5669105660389766</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>0.93003437900915742</v>
-      </c>
-      <c r="B70">
-        <v>0.73212371148153066</v>
-      </c>
-      <c r="C70">
-        <v>0.12861105403616291</v>
-      </c>
-      <c r="D70">
-        <v>0.12861105403616291</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>0.80312925251200795</v>
-      </c>
-      <c r="B71">
-        <v>0.27723276185663853</v>
-      </c>
-      <c r="C71">
-        <v>-0.65976582412958029</v>
-      </c>
-      <c r="D71">
-        <v>-0.65976582412958029</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>-0.68696849793195724</v>
-      </c>
-      <c r="B72">
-        <v>0.85646519989367853</v>
-      </c>
-      <c r="C72">
-        <v>2.4321500942923606</v>
-      </c>
-      <c r="D72">
-        <v>2.4321500942923606</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>-0.6590762953273952</v>
-      </c>
-      <c r="B73">
-        <v>0.87030137716759659</v>
-      </c>
-      <c r="C73">
-        <v>6.3744434583225544</v>
-      </c>
-      <c r="D73">
-        <v>6.3744434583225544</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>0.3168933866545558</v>
-      </c>
-      <c r="B74">
-        <v>0.88745993806447188</v>
-      </c>
-      <c r="C74">
-        <v>2.8505365823561846</v>
-      </c>
-      <c r="D74">
-        <v>2.8505365823561846</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>0.60784284537658095</v>
-      </c>
-      <c r="B75">
-        <v>0.71701165218701191</v>
-      </c>
-      <c r="C75">
-        <v>1.5461745982230135</v>
-      </c>
-      <c r="D75">
-        <v>1.5461745982230135</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>-0.59493754617869854</v>
-      </c>
-      <c r="B76">
-        <v>0.50830310050459138</v>
-      </c>
-      <c r="C76">
-        <v>2.3491970193892695</v>
-      </c>
-      <c r="D76">
-        <v>2.3491970193892695</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>0.27055360563099384</v>
-      </c>
-      <c r="B77">
-        <v>0.61967795842667939</v>
-      </c>
-      <c r="C77">
-        <v>1.8487862557860726</v>
-      </c>
-      <c r="D77">
-        <v>1.8487862557860726</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>-0.10009184200316668</v>
-      </c>
-      <c r="B78">
-        <v>0.24006192989349837</v>
-      </c>
-      <c r="C78">
-        <v>1.1935708685451325</v>
-      </c>
-      <c r="D78">
-        <v>1.1935708685451325</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>0.79606163268908858</v>
-      </c>
-      <c r="B79">
-        <v>0.45599108148897033</v>
-      </c>
-      <c r="C79">
-        <v>2.4149826706961917</v>
-      </c>
-      <c r="D79">
-        <v>2.4149826706961917</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>-0.33815954113379121</v>
-      </c>
-      <c r="B80">
-        <v>0.85066148317167645</v>
-      </c>
-      <c r="C80">
-        <v>5.1969840339901987</v>
-      </c>
-      <c r="D80">
-        <v>5.1969840339901987</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>-0.25958700757473707</v>
-      </c>
-      <c r="B81">
-        <v>0.60215006583329755</v>
-      </c>
-      <c r="C81">
-        <v>-1.9021269811673447</v>
-      </c>
-      <c r="D81">
-        <v>-1.9021269811673447</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>0.6611259076744318</v>
-      </c>
-      <c r="B82">
-        <v>0.74189061213826046</v>
-      </c>
-      <c r="C82">
-        <v>3.5767110282390639</v>
-      </c>
-      <c r="D82">
-        <v>3.5767110282390639</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>-0.4177185851149261</v>
-      </c>
-      <c r="B83">
-        <v>0.37432048000845114</v>
-      </c>
-      <c r="C83">
-        <v>1.1545554672128397</v>
-      </c>
-      <c r="D83">
-        <v>1.1545554672128397</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>0.62532191211357713</v>
-      </c>
-      <c r="B84">
-        <v>0.61941352062909771</v>
-      </c>
-      <c r="C84">
-        <v>-1.9089264363352179</v>
-      </c>
-      <c r="D84">
-        <v>-1.9089264363352179</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>0.28010437684133649</v>
-      </c>
-      <c r="B85">
-        <v>0.11187126962852734</v>
-      </c>
-      <c r="C85">
-        <v>4.1383001919165139</v>
-      </c>
-      <c r="D85">
-        <v>4.1383001919165139</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>0.37171070743352175</v>
-      </c>
-      <c r="B86">
-        <v>0.22914502905569734</v>
-      </c>
-      <c r="C86">
-        <v>-0.73538181680084413</v>
-      </c>
-      <c r="D86">
-        <v>-0.73538181680084413</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>-2.3498728405684233E-2</v>
-      </c>
-      <c r="B87">
-        <v>0.83423183832299708</v>
-      </c>
-      <c r="C87">
-        <v>6.1520467110905814</v>
-      </c>
-      <c r="D87">
-        <v>6.1520467110905814</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>0.36598141398280859</v>
-      </c>
-      <c r="B88">
-        <v>0.36052129017813928</v>
-      </c>
-      <c r="C88">
-        <v>3.0652817896660673</v>
-      </c>
-      <c r="D88">
-        <v>3.0652817896660673</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>-0.73137106746435165</v>
-      </c>
-      <c r="B89">
-        <v>0.9523209941081725</v>
-      </c>
-      <c r="C89">
-        <v>-1.2541605097835546</v>
-      </c>
-      <c r="D89">
-        <v>-1.2541605097835546</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <v>6.6931700333952904E-2</v>
-      </c>
-      <c r="B90">
-        <v>0.33932080191803249</v>
-      </c>
-      <c r="C90">
-        <v>2.8154014222675272</v>
-      </c>
-      <c r="D90">
-        <v>2.8154014222675272</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>0.50061998516321182</v>
-      </c>
-      <c r="B91">
-        <v>0.58717582933158641</v>
-      </c>
-      <c r="C91">
-        <v>3.0275562573791142</v>
-      </c>
-      <c r="D91">
-        <v>3.0275562573791142</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>0.25722116138786077</v>
-      </c>
-      <c r="B92">
-        <v>0.67185143525285274</v>
-      </c>
-      <c r="C92">
-        <v>5.6486916454667258</v>
-      </c>
-      <c r="D92">
-        <v>5.6486916454667258</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>-0.32637759391218424</v>
-      </c>
-      <c r="B93">
-        <v>0.65143113937539654</v>
-      </c>
-      <c r="C93">
-        <v>3.829135001119909</v>
-      </c>
-      <c r="D93">
-        <v>3.829135001119909</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>-0.801655865740031</v>
-      </c>
-      <c r="B94">
-        <v>0.37540367192598789</v>
-      </c>
-      <c r="C94">
-        <v>7.784545404301034</v>
-      </c>
-      <c r="D94">
-        <v>7.784545404301034</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>0.79797026654705405</v>
-      </c>
-      <c r="B95">
-        <v>0.87009751405998814</v>
-      </c>
-      <c r="C95">
-        <v>-2.4411080132540901</v>
-      </c>
-      <c r="D95">
-        <v>-2.4411080132540901</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>6.05545649304986E-2</v>
-      </c>
-      <c r="B96">
-        <v>0.83226891657592039</v>
-      </c>
-      <c r="C96">
-        <v>5.7577909822258997</v>
-      </c>
-      <c r="D96">
-        <v>5.7577909822258997</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97">
-        <v>-0.80952635360881686</v>
-      </c>
-      <c r="B97">
-        <v>0.3199582956942279</v>
-      </c>
-      <c r="C97">
-        <v>-1.4940430248515804</v>
-      </c>
-      <c r="D97">
-        <v>-1.4940430248515804</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98">
-        <v>0.45351168466731906</v>
-      </c>
-      <c r="B98">
-        <v>0.49291685043121797</v>
-      </c>
-      <c r="C98">
-        <v>0.15100594179886162</v>
-      </c>
-      <c r="D98">
-        <v>0.15100594179886162</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99">
-        <v>0.34591140458360314</v>
-      </c>
-      <c r="B99">
-        <v>0.38765161365002254</v>
-      </c>
-      <c r="C99">
-        <v>2.6161221467094253</v>
-      </c>
-      <c r="D99">
-        <v>2.6161221467094253</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>0.7174810110591352</v>
-      </c>
-      <c r="B100">
-        <v>0.82573982937149881</v>
-      </c>
-      <c r="C100">
-        <v>4.9221390967172383</v>
-      </c>
-      <c r="D100">
-        <v>4.9221390967172383</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <v>-0.94411851745098829</v>
-      </c>
-      <c r="B101">
-        <v>0.90323890173730392</v>
-      </c>
-      <c r="C101">
-        <v>4.0263725186965367</v>
-      </c>
-      <c r="D101">
-        <v>4.0263725186965367</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>